<commit_message>
Add Changes to BSR Analysis Script (Takes One More Command Line Argument)
</commit_message>
<xml_diff>
--- a/BSR analysis/re.xlsx
+++ b/BSR analysis/re.xlsx
@@ -11,6 +11,165 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+  <si>
+    <t>['ABM', 'CAM', 'KEP']</t>
+  </si>
+  <si>
+    <t>ABM12334</t>
+  </si>
+  <si>
+    <t>Uncharacterized protein</t>
+  </si>
+  <si>
+    <t>[' DUF4349.']</t>
+  </si>
+  <si>
+    <t>[' DUF4349']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>KEP40542</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>CAM63497</t>
+  </si>
+  <si>
+    <t>['ABK', 'ABM', 'CAM', 'CAR', 'EJZ', 'ETA']</t>
+  </si>
+  <si>
+    <t>CAR70428</t>
+  </si>
+  <si>
+    <t>Putative ABC-transporter transmembrane protein</t>
+  </si>
+  <si>
+    <t>[' ABC_3.', ' ABC_BtuC-like.']</t>
+  </si>
+  <si>
+    <t>[' ABC-3']</t>
+  </si>
+  <si>
+    <t>ATPase activity, coupled to transmembrane movement of substances</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ATP binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> integral component of membrane
+</t>
+  </si>
+  <si>
+    <t>ABM16089</t>
+  </si>
+  <si>
+    <t>ABC-3 protein</t>
+  </si>
+  <si>
+    <t>ABK71462</t>
+  </si>
+  <si>
+    <t>ABC heavy metal transporter, inner membrane subunit (ABC-3)</t>
+  </si>
+  <si>
+    <t>ETA91263</t>
+  </si>
+  <si>
+    <t>Helicase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> helicase activity</t>
+  </si>
+  <si>
+    <t>EJZ09704</t>
+  </si>
+  <si>
+    <t>CAM60673</t>
+  </si>
+  <si>
+    <t>['ABK', 'ABM', 'CAM', 'CAR', 'EJZ', 'ETA', 'KEP', 'TUB']</t>
+  </si>
+  <si>
+    <t>KEP42447</t>
+  </si>
+  <si>
+    <t>Shikimate 5-dehydrogenase</t>
+  </si>
+  <si>
+    <t>CAR70608</t>
+  </si>
+  <si>
+    <t>Putative shikimate 5-dehydrogenase</t>
+  </si>
+  <si>
+    <t>[' NAD(P)-bd_dom.', ' Shikimate_DH-bd_N.', ' Shikimate_DH_AroM-type.']</t>
+  </si>
+  <si>
+    <t>[' Shikimate_dh_N']</t>
+  </si>
+  <si>
+    <t>cytoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shikimate 3-dehydrogenase (NADP+) activity
+</t>
+  </si>
+  <si>
+    <t>ABM13451</t>
+  </si>
+  <si>
+    <t>Shikimate-5-dehydrogenase</t>
+  </si>
+  <si>
+    <t>[' NAD(P)-bd_dom.', ' Shikimate_DH-bd_N.', ' Shikimate_DH_AroM-type.', ' Shikm_DH/Glu-tRNA_Rdtase.']</t>
+  </si>
+  <si>
+    <t>[' Shikimate_DH', ' Shikimate_dh_N']</t>
+  </si>
+  <si>
+    <t>ABK75112</t>
+  </si>
+  <si>
+    <t>Shikimate 5-dehydrogenase (Shikimate dehydrogenase substrate binding domain protein) (EC 1.1.1.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shikimate 3-dehydrogenase (NADP+) activity
+</t>
+  </si>
+  <si>
+    <t>EJZ07380</t>
+  </si>
+  <si>
+    <t>Shikimate 5-dehydrogenase (EC 1.1.1.25)</t>
+  </si>
+  <si>
+    <t>[' NAD(P)-bd_dom.', ' Shikimate_DH-bd_N.', ' Shikm_DH/Glu-tRNA_Rdtase.']</t>
+  </si>
+  <si>
+    <t>ABM15590</t>
+  </si>
+  <si>
+    <t>Shikimate dehydrogenase (EC 1.1.1.25)</t>
+  </si>
+  <si>
+    <t>[' NAD(P)-bd_dom.', ' Shikimate_DH-bd_N.']</t>
+  </si>
+  <si>
+    <t>EJZ11959</t>
+  </si>
+  <si>
+    <t>TUB57484</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +499,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>